<commit_message>
Fikset sånn at den printer alle SNR
</commit_message>
<xml_diff>
--- a/innafor.xlsx
+++ b/innafor.xlsx
@@ -19,7 +19,7 @@
     <t>FFT Length</t>
   </si>
   <si>
-    <t>SNR</t>
+    <t>SNR [dB]</t>
   </si>
   <si>
     <t>Mean estimated</t>
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,6 +411,9 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>-10</v>
+      </c>
       <c r="C2">
         <v>99609.375</v>
       </c>
@@ -425,6 +428,9 @@
       </c>
     </row>
     <row r="3" spans="1:6">
+      <c r="B3">
+        <v>0</v>
+      </c>
       <c r="C3">
         <v>99609.375</v>
       </c>
@@ -439,6 +445,9 @@
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="B4">
+        <v>10</v>
+      </c>
       <c r="C4">
         <v>99609.375</v>
       </c>
@@ -453,6 +462,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="B5">
+        <v>20</v>
+      </c>
       <c r="C5">
         <v>99609.375</v>
       </c>
@@ -467,82 +479,97 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="B6">
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>99975.5859375</v>
+        <v>99609.375</v>
       </c>
       <c r="D6">
-        <v>24.4140625</v>
+        <v>390.625</v>
       </c>
       <c r="E6">
-        <v>29802.32238769531</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>444427.3784331126</v>
+        <v>44.44273784331126</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="B7">
+        <v>40</v>
+      </c>
       <c r="C7">
-        <v>99975.5859375</v>
+        <v>99609.375</v>
       </c>
       <c r="D7">
-        <v>24.4140625</v>
+        <v>390.625</v>
       </c>
       <c r="E7">
-        <v>29802.32238769531</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>44442.73784331126</v>
+        <v>4.444273784331127</v>
       </c>
     </row>
     <row r="8" spans="1:6">
+      <c r="B8">
+        <v>50</v>
+      </c>
       <c r="C8">
-        <v>100097.65625</v>
+        <v>99609.375</v>
       </c>
       <c r="D8">
-        <v>-97.65625</v>
+        <v>390.625</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>4444.273784331127</v>
+        <v>0.4444273784331127</v>
       </c>
     </row>
     <row r="9" spans="1:6">
+      <c r="B9">
+        <v>60</v>
+      </c>
       <c r="C9">
-        <v>100097.65625</v>
+        <v>99609.375</v>
       </c>
       <c r="D9">
-        <v>-97.65625</v>
+        <v>390.625</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>444.4273784331126</v>
+        <v>0.04444273784331126</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>-10</v>
       </c>
       <c r="C10">
-        <v>100067.138671875</v>
+        <v>100097.65625</v>
       </c>
       <c r="D10">
-        <v>-67.138671875</v>
+        <v>-97.65625</v>
       </c>
       <c r="E10">
-        <v>1862.645149230957</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>444427.3784331126</v>
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
         <v>99975.5859375</v>
       </c>
@@ -550,32 +577,38 @@
         <v>24.4140625</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>29802.32238769531</v>
       </c>
       <c r="F11">
         <v>44442.73784331126</v>
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="B12">
+        <v>10</v>
+      </c>
       <c r="C12">
-        <v>100006.103515625</v>
+        <v>100097.65625</v>
       </c>
       <c r="D12">
-        <v>-6.103515625</v>
+        <v>-97.65625</v>
       </c>
       <c r="E12">
-        <v>1862.645149230957</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>4444.273784331127</v>
       </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="B13">
+        <v>20</v>
+      </c>
       <c r="C13">
-        <v>99975.5859375</v>
+        <v>100097.65625</v>
       </c>
       <c r="D13">
-        <v>24.4140625</v>
+        <v>-97.65625</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -585,235 +618,626 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>9</v>
+      <c r="B14">
+        <v>30</v>
       </c>
       <c r="C14">
-        <v>99975.5859375</v>
+        <v>100097.65625</v>
       </c>
       <c r="D14">
-        <v>24.4140625</v>
+        <v>-97.65625</v>
       </c>
       <c r="E14">
-        <v>11641.53218269348</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>444427.3784331126</v>
+        <v>44.44273784331126</v>
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="B15">
+        <v>40</v>
+      </c>
       <c r="C15">
-        <v>99990.8447265625</v>
+        <v>100097.65625</v>
       </c>
       <c r="D15">
-        <v>9.1552734375</v>
+        <v>-97.65625</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>44442.73784331126</v>
+        <v>4.444273784331127</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="B16">
+        <v>50</v>
+      </c>
       <c r="C16">
-        <v>100006.103515625</v>
+        <v>100097.65625</v>
       </c>
       <c r="D16">
-        <v>-6.103515625</v>
+        <v>-97.65625</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>4444.273784331127</v>
+        <v>0.4444273784331127</v>
       </c>
     </row>
     <row r="17" spans="1:6">
+      <c r="B17">
+        <v>60</v>
+      </c>
       <c r="C17">
-        <v>99998.47412109375</v>
+        <v>100097.65625</v>
       </c>
       <c r="D17">
-        <v>1.52587890625</v>
+        <v>-97.65625</v>
       </c>
       <c r="E17">
-        <v>116.4153218269348</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>444.4273784331126</v>
+        <v>0.04444273784331126</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>-10</v>
       </c>
       <c r="C18">
-        <v>100111.0076904297</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D18">
-        <v>-111.0076904296875</v>
+        <v>24.4140625</v>
       </c>
       <c r="E18">
-        <v>2626.620698720217</v>
+        <v>29802.32238769531</v>
       </c>
       <c r="F18">
         <v>444427.3784331126</v>
       </c>
     </row>
     <row r="19" spans="1:6">
+      <c r="B19">
+        <v>0</v>
+      </c>
       <c r="C19">
-        <v>99987.03002929688</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D19">
-        <v>12.969970703125</v>
+        <v>24.4140625</v>
       </c>
       <c r="E19">
-        <v>727.5957614183426</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>44442.73784331126</v>
       </c>
     </row>
     <row r="20" spans="1:6">
+      <c r="B20">
+        <v>10</v>
+      </c>
       <c r="C20">
-        <v>99998.47412109375</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D20">
-        <v>1.52587890625</v>
+        <v>24.4140625</v>
       </c>
       <c r="E20">
-        <v>116.4153218269348</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>4444.273784331127</v>
       </c>
     </row>
     <row r="21" spans="1:6">
+      <c r="B21">
+        <v>20</v>
+      </c>
       <c r="C21">
-        <v>99996.56677246094</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D21">
-        <v>3.4332275390625</v>
+        <v>24.4140625</v>
       </c>
       <c r="E21">
-        <v>7.275957614183426</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>444.4273784331126</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>99975.5859375</v>
+      </c>
+      <c r="D22">
+        <v>24.4140625</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>44.44273784331126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>99975.5859375</v>
+      </c>
+      <c r="D23">
+        <v>24.4140625</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>4.444273784331127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>99975.5859375</v>
+      </c>
+      <c r="D24">
+        <v>24.4140625</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0.4444273784331127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>99975.5859375</v>
+      </c>
+      <c r="D25">
+        <v>24.4140625</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0.04444273784331126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>-10</v>
+      </c>
+      <c r="C26">
+        <v>99952.69775390625</v>
+      </c>
+      <c r="D26">
+        <v>47.30224609375</v>
+      </c>
+      <c r="E26">
+        <v>33644.02800798416</v>
+      </c>
+      <c r="F26">
+        <v>444427.3784331126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>100013.7329101562</v>
+      </c>
+      <c r="D27">
+        <v>-13.73291015625</v>
+      </c>
+      <c r="E27">
+        <v>1047.737896442413</v>
+      </c>
+      <c r="F27">
+        <v>44442.73784331126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>99998.47412109375</v>
+      </c>
+      <c r="D28">
+        <v>1.52587890625</v>
+      </c>
+      <c r="E28">
+        <v>116.4153218269348</v>
+      </c>
+      <c r="F28">
+        <v>4444.273784331127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>100006.103515625</v>
+      </c>
+      <c r="D29">
+        <v>-6.103515625</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>444.4273784331126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>100006.103515625</v>
+      </c>
+      <c r="D30">
+        <v>-6.103515625</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>44.44273784331126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>100006.103515625</v>
+      </c>
+      <c r="D31">
+        <v>-6.103515625</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>4.444273784331127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="B32">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>100006.103515625</v>
+      </c>
+      <c r="D32">
+        <v>-6.103515625</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0.4444273784331127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>100006.103515625</v>
+      </c>
+      <c r="D33">
+        <v>-6.103515625</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0.04444273784331126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>-10</v>
+      </c>
+      <c r="C34">
+        <v>100055.6945800781</v>
+      </c>
+      <c r="D34">
+        <v>-55.694580078125</v>
+      </c>
+      <c r="E34">
+        <v>116.4153218269348</v>
+      </c>
+      <c r="F34">
+        <v>444427.3784331126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>99967.95654296875</v>
+      </c>
+      <c r="D35">
+        <v>32.04345703125</v>
+      </c>
+      <c r="E35">
+        <v>261.9344741106033</v>
+      </c>
+      <c r="F35">
+        <v>44442.73784331126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>99998.47412109375</v>
+      </c>
+      <c r="D36">
+        <v>1.52587890625</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>4444.273784331127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>100000.3814697266</v>
+      </c>
+      <c r="D37">
+        <v>-0.3814697265625</v>
+      </c>
+      <c r="E37">
+        <v>7.275957614183426</v>
+      </c>
+      <c r="F37">
+        <v>444.4273784331126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>100000.3814697266</v>
+      </c>
+      <c r="D38">
+        <v>-0.3814697265625</v>
+      </c>
+      <c r="E38">
+        <v>7.275957614183426</v>
+      </c>
+      <c r="F38">
+        <v>44.44273784331126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="B39">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>99998.47412109375</v>
+      </c>
+      <c r="D39">
+        <v>1.52587890625</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>4.444273784331127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="B40">
+        <v>50</v>
+      </c>
+      <c r="C40">
+        <v>99998.47412109375</v>
+      </c>
+      <c r="D40">
+        <v>1.52587890625</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.4444273784331127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41">
+        <v>60</v>
+      </c>
+      <c r="C41">
+        <v>99998.47412109375</v>
+      </c>
+      <c r="D41">
+        <v>1.52587890625</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0.04444273784331126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="C22">
+      <c r="B42">
+        <v>-10</v>
+      </c>
+      <c r="C42">
+        <v>100035.1905822754</v>
+      </c>
+      <c r="D42">
+        <v>-35.19058227539062</v>
+      </c>
+      <c r="E42">
+        <v>164.1637936700135</v>
+      </c>
+      <c r="F42">
+        <v>444427.3784331126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>99988.93737792969</v>
+      </c>
+      <c r="D43">
+        <v>11.0626220703125</v>
+      </c>
+      <c r="E43">
+        <v>465.6612873077393</v>
+      </c>
+      <c r="F43">
+        <v>44442.73784331126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>100003.2424926758</v>
+      </c>
+      <c r="D44">
+        <v>-3.24249267578125</v>
+      </c>
+      <c r="E44">
+        <v>45.47473508864641</v>
+      </c>
+      <c r="F44">
+        <v>4444.273784331127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>100003.2424926758</v>
+      </c>
+      <c r="D45">
+        <v>-3.24249267578125</v>
+      </c>
+      <c r="E45">
+        <v>1.818989403545856</v>
+      </c>
+      <c r="F45">
+        <v>444.4273784331126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="B46">
+        <v>30</v>
+      </c>
+      <c r="C46">
         <v>99999.42779541016</v>
       </c>
-      <c r="D22">
+      <c r="D46">
         <v>0.57220458984375</v>
       </c>
-      <c r="E22">
-        <v>13142.19844061881</v>
-      </c>
-      <c r="F22">
-        <v>444427.3784331126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="C23">
-        <v>99988.93737792969</v>
-      </c>
-      <c r="D23">
-        <v>11.0626220703125</v>
-      </c>
-      <c r="E23">
-        <v>7.275957614183426</v>
-      </c>
-      <c r="F23">
-        <v>44442.73784331126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="C24">
-        <v>100004.1961669922</v>
-      </c>
-      <c r="D24">
-        <v>-4.1961669921875</v>
-      </c>
-      <c r="E24">
-        <v>16.37090463191271</v>
-      </c>
-      <c r="F24">
-        <v>4444.273784331127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="C25">
-        <v>100000.8583068848</v>
-      </c>
-      <c r="D25">
-        <v>-0.858306884765625</v>
-      </c>
-      <c r="E25">
-        <v>22.28262019343674</v>
-      </c>
-      <c r="F25">
-        <v>444.4273784331126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="C26">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>44.44273784331126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47">
+        <v>40</v>
+      </c>
+      <c r="C47">
+        <v>99999.90463256836</v>
+      </c>
+      <c r="D47">
+        <v>0.095367431640625</v>
+      </c>
+      <c r="E47">
+        <v>0.4547473508864641</v>
+      </c>
+      <c r="F47">
+        <v>4.444273784331127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="B48">
+        <v>50</v>
+      </c>
+      <c r="C48">
         <v>100000.3814697266</v>
       </c>
-      <c r="D26">
+      <c r="D48">
         <v>-0.3814697265625</v>
       </c>
-      <c r="E26">
-        <v>1.818989403545856</v>
-      </c>
-      <c r="F26">
-        <v>44.44273784331126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="C27">
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0.4444273784331127</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49">
+        <v>60</v>
+      </c>
+      <c r="C49">
         <v>100000.3814697266</v>
       </c>
-      <c r="D27">
+      <c r="D49">
         <v>-0.3814697265625</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>4.444273784331127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="C28">
-        <v>100000.3814697266</v>
-      </c>
-      <c r="D28">
-        <v>-0.3814697265625</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0.4444273784331127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="C29">
-        <v>100000.3814697266</v>
-      </c>
-      <c r="D29">
-        <v>-0.3814697265625</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
         <v>0.04444273784331126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed variance estimation & CRLB
</commit_message>
<xml_diff>
--- a/innafor.xlsx
+++ b/innafor.xlsx
@@ -31,7 +31,7 @@
     <t>Variance</t>
   </si>
   <si>
-    <t>CRLB</t>
+    <t>CRLB [Hz^2]</t>
   </si>
   <si>
     <t>1024</t>
@@ -415,16 +415,16 @@
         <v>-10</v>
       </c>
       <c r="C2">
-        <v>99804.6875</v>
+        <v>99707.03125</v>
       </c>
       <c r="D2">
-        <v>195.3125</v>
+        <v>292.96875</v>
       </c>
       <c r="E2">
-        <v>154129.182449495</v>
+        <v>95367.431640625</v>
       </c>
       <c r="F2">
-        <v>444427.3784331126</v>
+        <v>22514.95401295208</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -441,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>44442.73784331126</v>
+        <v>2251.495401295208</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>4444.273784331127</v>
+        <v>225.1495401295208</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>444.4273784331126</v>
+        <v>22.51495401295207</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>44.44273784331126</v>
+        <v>2.251495401295208</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>4.444273784331127</v>
+        <v>0.2251495401295208</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.4444273784331127</v>
+        <v>0.02251495401295208</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.04444273784331126</v>
+        <v>0.002251495401295208</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -554,16 +554,16 @@
         <v>-10</v>
       </c>
       <c r="C10">
-        <v>100019.53125</v>
+        <v>99926.7578125</v>
       </c>
       <c r="D10">
-        <v>-19.53125</v>
+        <v>73.2421875</v>
       </c>
       <c r="E10">
-        <v>19121.65169764047</v>
+        <v>27153.22706434462</v>
       </c>
       <c r="F10">
-        <v>444427.3784331126</v>
+        <v>22514.95401295208</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -571,16 +571,16 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>100043.9453125</v>
+        <v>100048.828125</v>
       </c>
       <c r="D11">
-        <v>-43.9453125</v>
+        <v>-48.828125</v>
       </c>
       <c r="E11">
-        <v>10331.47176106771</v>
+        <v>10596.38129340278</v>
       </c>
       <c r="F11">
-        <v>44442.73784331126</v>
+        <v>2251.495401295208</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -588,16 +588,16 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>100095.21484375</v>
+        <v>100073.2421875</v>
       </c>
       <c r="D12">
-        <v>-95.21484375</v>
+        <v>-73.2421875</v>
       </c>
       <c r="E12">
-        <v>596.0464477539062</v>
+        <v>5960.464477539062</v>
       </c>
       <c r="F12">
-        <v>4444.273784331127</v>
+        <v>225.1495401295208</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>444.4273784331126</v>
+        <v>22.51495401295207</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>44.44273784331126</v>
+        <v>2.251495401295208</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>4.444273784331127</v>
+        <v>0.2251495401295208</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.4444273784331127</v>
+        <v>0.02251495401295208</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.04444273784331126</v>
+        <v>0.002251495401295208</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -693,16 +693,16 @@
         <v>-10</v>
       </c>
       <c r="C18">
-        <v>100012.20703125</v>
+        <v>99981.689453125</v>
       </c>
       <c r="D18">
-        <v>-12.20703125</v>
+        <v>18.310546875</v>
       </c>
       <c r="E18">
-        <v>13320.73500662139</v>
+        <v>12790.16335805257</v>
       </c>
       <c r="F18">
-        <v>444427.3784331126</v>
+        <v>22514.95401295208</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -710,16 +710,16 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>99997.55859375</v>
+        <v>100000</v>
       </c>
       <c r="D19">
-        <v>2.44140625</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1243.268600617996</v>
+        <v>1821.253034803603</v>
       </c>
       <c r="F19">
-        <v>44442.73784331126</v>
+        <v>2251.495401295208</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -733,10 +733,10 @@
         <v>6.103515625</v>
       </c>
       <c r="E20">
-        <v>790.2130936131333</v>
+        <v>869.2344029744467</v>
       </c>
       <c r="F20">
-        <v>4444.273784331127</v>
+        <v>225.1495401295208</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -744,16 +744,16 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>99976.806640625</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D21">
-        <v>23.193359375</v>
+        <v>24.4140625</v>
       </c>
       <c r="E21">
-        <v>73.7532220705591</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>444.4273784331126</v>
+        <v>22.51495401295207</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>44.44273784331126</v>
+        <v>2.251495401295208</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>4.444273784331127</v>
+        <v>0.2251495401295208</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0.4444273784331127</v>
+        <v>0.02251495401295208</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0.04444273784331126</v>
+        <v>0.002251495401295208</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -832,16 +832,16 @@
         <v>-10</v>
       </c>
       <c r="C26">
-        <v>99980.62133789062</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D26">
-        <v>19.378662109375</v>
+        <v>24.4140625</v>
       </c>
       <c r="E26">
-        <v>13146.958680767</v>
+        <v>16142.92462666829</v>
       </c>
       <c r="F26">
-        <v>444427.3784331126</v>
+        <v>22514.95401295208</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -849,16 +849,16 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>99992.82836914062</v>
+        <v>99986.26708984375</v>
       </c>
       <c r="D27">
-        <v>7.171630859375</v>
+        <v>13.73291015625</v>
       </c>
       <c r="E27">
-        <v>1258.95527125609</v>
+        <v>1606.5314412117</v>
       </c>
       <c r="F27">
-        <v>44442.73784331126</v>
+        <v>2251.495401295208</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -866,16 +866,16 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>100000.1525878906</v>
+        <v>100000</v>
       </c>
       <c r="D28">
-        <v>-0.152587890625</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>145.3192471855819</v>
+        <v>62.0881716410319</v>
       </c>
       <c r="F28">
-        <v>4444.273784331127</v>
+        <v>225.1495401295208</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -883,16 +883,16 @@
         <v>20</v>
       </c>
       <c r="C29">
-        <v>100000.9155273438</v>
+        <v>100001.5258789062</v>
       </c>
       <c r="D29">
-        <v>-0.91552734375</v>
+        <v>-1.52587890625</v>
       </c>
       <c r="E29">
-        <v>52.77494589487711</v>
+        <v>54.32715018590292</v>
       </c>
       <c r="F29">
-        <v>444.4273784331126</v>
+        <v>22.51495401295207</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -900,16 +900,16 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>100004.4250488281</v>
+        <v>100004.5776367188</v>
       </c>
       <c r="D30">
-        <v>-4.425048828125</v>
+        <v>-4.57763671875</v>
       </c>
       <c r="E30">
-        <v>23.024363650216</v>
+        <v>23.28306436538696</v>
       </c>
       <c r="F30">
-        <v>44.44273784331126</v>
+        <v>2.251495401295208</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>4.444273784331127</v>
+        <v>0.2251495401295208</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.4444273784331127</v>
+        <v>0.02251495401295208</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.04444273784331126</v>
+        <v>0.002251495401295208</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -971,16 +971,16 @@
         <v>-10</v>
       </c>
       <c r="C34">
-        <v>99996.49047851562</v>
+        <v>99993.51501464844</v>
       </c>
       <c r="D34">
-        <v>3.509521484375</v>
+        <v>6.4849853515625</v>
       </c>
       <c r="E34">
-        <v>10466.93686282996</v>
+        <v>6645.536308901177</v>
       </c>
       <c r="F34">
-        <v>444427.3784331126</v>
+        <v>22514.95401295208</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -988,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>99999.61853027344</v>
+        <v>99986.26708984375</v>
       </c>
       <c r="D35">
-        <v>0.3814697265625</v>
+        <v>13.73291015625</v>
       </c>
       <c r="E35">
-        <v>867.6763191217124</v>
+        <v>785.1566705438826</v>
       </c>
       <c r="F35">
-        <v>44442.73784331126</v>
+        <v>2251.495401295208</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1005,16 +1005,16 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>100003.3569335938</v>
+        <v>99998.09265136719</v>
       </c>
       <c r="D36">
-        <v>-3.35693359375</v>
+        <v>1.9073486328125</v>
       </c>
       <c r="E36">
-        <v>104.973694742328</v>
+        <v>127.5717901686827</v>
       </c>
       <c r="F36">
-        <v>4444.273784331127</v>
+        <v>225.1495401295208</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1022,16 +1022,16 @@
         <v>20</v>
       </c>
       <c r="C37">
-        <v>99999.73297119141</v>
+        <v>100001.1444091797</v>
       </c>
       <c r="D37">
-        <v>0.26702880859375</v>
+        <v>-1.1444091796875</v>
       </c>
       <c r="E37">
-        <v>12.9512045532465</v>
+        <v>9.862964765893089</v>
       </c>
       <c r="F37">
-        <v>444.4273784331126</v>
+        <v>22.51495401295207</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1039,16 +1039,16 @@
         <v>30</v>
       </c>
       <c r="C38">
-        <v>99999.73297119141</v>
+        <v>100000.3814697266</v>
       </c>
       <c r="D38">
-        <v>0.26702880859375</v>
+        <v>-0.3814697265625</v>
       </c>
       <c r="E38">
-        <v>3.249927734335264</v>
+        <v>4.042198674546348</v>
       </c>
       <c r="F38">
-        <v>44.44273784331126</v>
+        <v>2.251495401295208</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1056,16 +1056,16 @@
         <v>40</v>
       </c>
       <c r="C39">
-        <v>99998.81744384766</v>
+        <v>99998.85559082031</v>
       </c>
       <c r="D39">
-        <v>1.18255615234375</v>
+        <v>1.1444091796875</v>
       </c>
       <c r="E39">
-        <v>1.203840259801258</v>
+        <v>1.455191522836685</v>
       </c>
       <c r="F39">
-        <v>4.444273784331127</v>
+        <v>0.2251495401295208</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.4444273784331127</v>
+        <v>0.02251495401295208</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.04444273784331126</v>
+        <v>0.002251495401295208</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1110,16 +1110,16 @@
         <v>-10</v>
       </c>
       <c r="C42">
-        <v>100013.4754180908</v>
+        <v>99978.82843017578</v>
       </c>
       <c r="D42">
-        <v>-13.47541809082031</v>
+        <v>21.17156982421875</v>
       </c>
       <c r="E42">
-        <v>9708.439870566986</v>
+        <v>14842.99395492093</v>
       </c>
       <c r="F42">
-        <v>444427.3784331126</v>
+        <v>22514.95401295208</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1127,16 +1127,16 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>100001.106262207</v>
+        <v>99973.0110168457</v>
       </c>
       <c r="D43">
-        <v>-1.10626220703125</v>
+        <v>26.98898315429688</v>
       </c>
       <c r="E43">
-        <v>1080.849383148656</v>
+        <v>988.3276814232684</v>
       </c>
       <c r="F43">
-        <v>44442.73784331126</v>
+        <v>2251.495401295208</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1144,16 +1144,16 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>100000.1907348633</v>
+        <v>99995.04089355469</v>
       </c>
       <c r="D44">
-        <v>-0.19073486328125</v>
+        <v>4.9591064453125</v>
       </c>
       <c r="E44">
-        <v>145.8315039994289</v>
+        <v>174.2591848596931</v>
       </c>
       <c r="F44">
-        <v>4444.273784331127</v>
+        <v>225.1495401295208</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1167,10 +1167,10 @@
         <v>0.095367431640625</v>
       </c>
       <c r="E45">
-        <v>10.44540884763454</v>
+        <v>16.82565198279917</v>
       </c>
       <c r="F45">
-        <v>444.4273784331126</v>
+        <v>22.51495401295207</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1178,16 +1178,16 @@
         <v>30</v>
       </c>
       <c r="C46">
-        <v>100000</v>
+        <v>100000.2861022949</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>-0.286102294921875</v>
       </c>
       <c r="E46">
-        <v>1.286154123719292</v>
+        <v>1.303609072541197</v>
       </c>
       <c r="F46">
-        <v>44.44273784331126</v>
+        <v>2.251495401295208</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1195,16 +1195,16 @@
         <v>40</v>
       </c>
       <c r="C47">
-        <v>99999.95231628418</v>
+        <v>99999.80926513672</v>
       </c>
       <c r="D47">
-        <v>0.0476837158203125</v>
+        <v>0.19073486328125</v>
       </c>
       <c r="E47">
-        <v>0.2273736754432321</v>
+        <v>0.2425319204727809</v>
       </c>
       <c r="F47">
-        <v>4.444273784331127</v>
+        <v>0.2251495401295208</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1212,16 +1212,16 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>100000.1049041748</v>
+        <v>100000.1907348633</v>
       </c>
       <c r="D48">
-        <v>-0.1049041748046875</v>
+        <v>-0.19073486328125</v>
       </c>
       <c r="E48">
-        <v>0.1891565243384302</v>
+        <v>0.1616879469818539</v>
       </c>
       <c r="F48">
-        <v>0.4444273784331127</v>
+        <v>0.02251495401295208</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -1229,16 +1229,16 @@
         <v>60</v>
       </c>
       <c r="C49">
-        <v>100000.3719329834</v>
+        <v>100000.3814697266</v>
       </c>
       <c r="D49">
-        <v>-0.3719329833984375</v>
+        <v>-0.3814697265625</v>
       </c>
       <c r="E49">
-        <v>0.009094947017729282</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>0.04444273784331126</v>
+        <v>0.002251495401295208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
la til 2^2 i CRLB2
</commit_message>
<xml_diff>
--- a/innafor.xlsx
+++ b/innafor.xlsx
@@ -415,16 +415,16 @@
         <v>-10</v>
       </c>
       <c r="C2">
-        <v>99863.28125</v>
+        <v>99787.109375</v>
       </c>
       <c r="D2">
-        <v>136.71875</v>
+        <v>212.890625</v>
       </c>
       <c r="E2">
-        <v>185340.3418955177</v>
+        <v>142121.338868165</v>
       </c>
       <c r="F2">
-        <v>22514.95401295208</v>
+        <v>11257.47700647604</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -441,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>2251.495401295208</v>
+        <v>1125.747700647604</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>225.1495401295208</v>
+        <v>112.5747700647604</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>22.51495401295207</v>
+        <v>11.25747700647604</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>2.251495401295208</v>
+        <v>1.125747700647604</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -509,7 +509,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.2251495401295208</v>
+        <v>0.1125747700647604</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0.02251495401295208</v>
+        <v>0.01125747700647604</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.002251495401295208</v>
+        <v>0.001125747700647604</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -554,16 +554,16 @@
         <v>-10</v>
       </c>
       <c r="C10">
-        <v>99992.67578125</v>
+        <v>99991.69921875</v>
       </c>
       <c r="D10">
-        <v>7.32421875</v>
+        <v>8.30078125</v>
       </c>
       <c r="E10">
-        <v>15960.79932318793</v>
+        <v>19309.99564933586</v>
       </c>
       <c r="F10">
-        <v>22514.95401295208</v>
+        <v>11257.47700647604</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -571,16 +571,16 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>100051.26953125</v>
+        <v>100040.771484375</v>
       </c>
       <c r="D11">
-        <v>-51.26953125</v>
+        <v>-40.771484375</v>
       </c>
       <c r="E11">
-        <v>9265.812960537996</v>
+        <v>10662.66834079563</v>
       </c>
       <c r="F11">
-        <v>2251.495401295208</v>
+        <v>1125.747700647604</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -588,16 +588,16 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>100097.65625</v>
+        <v>100094.970703125</v>
       </c>
       <c r="D12">
-        <v>-97.65625</v>
+        <v>-94.970703125</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>649.0880185300047</v>
       </c>
       <c r="F12">
-        <v>225.1495401295208</v>
+        <v>112.5747700647604</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>22.51495401295207</v>
+        <v>11.25747700647604</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>2.251495401295208</v>
+        <v>1.125747700647604</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0.2251495401295208</v>
+        <v>0.1125747700647604</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0.02251495401295208</v>
+        <v>0.01125747700647604</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0.002251495401295208</v>
+        <v>0.001125747700647604</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -693,16 +693,16 @@
         <v>-10</v>
       </c>
       <c r="C18">
-        <v>100007.32421875</v>
+        <v>99999.51171875</v>
       </c>
       <c r="D18">
-        <v>-7.32421875</v>
+        <v>0.48828125</v>
       </c>
       <c r="E18">
-        <v>12905.30869455049</v>
+        <v>11449.34225607443</v>
       </c>
       <c r="F18">
-        <v>22514.95401295208</v>
+        <v>11257.47700647604</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -710,16 +710,16 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>100004.8828125</v>
+        <v>100000.0610351562</v>
       </c>
       <c r="D19">
-        <v>-4.8828125</v>
+        <v>-0.06103515625</v>
       </c>
       <c r="E19">
-        <v>1691.808604230784</v>
+        <v>1552.014111040591</v>
       </c>
       <c r="F19">
-        <v>2251.495401295208</v>
+        <v>1125.747700647604</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -727,16 +727,16 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <v>99991.455078125</v>
+        <v>99993.5302734375</v>
       </c>
       <c r="D20">
-        <v>8.544921875</v>
+        <v>6.4697265625</v>
       </c>
       <c r="E20">
-        <v>723.985710529366</v>
+        <v>774.0101656756243</v>
       </c>
       <c r="F20">
-        <v>225.1495401295208</v>
+        <v>112.5747700647604</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -744,16 +744,16 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <v>99975.5859375</v>
+        <v>99977.72216796875</v>
       </c>
       <c r="D21">
-        <v>24.4140625</v>
+        <v>22.27783203125</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>125.9476274580092</v>
       </c>
       <c r="F21">
-        <v>22.51495401295207</v>
+        <v>11.25747700647604</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>2.251495401295208</v>
+        <v>1.125747700647604</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0.2251495401295208</v>
+        <v>0.1125747700647604</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -804,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0.02251495401295208</v>
+        <v>0.01125747700647604</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0.002251495401295208</v>
+        <v>0.001125747700647604</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -832,16 +832,16 @@
         <v>-10</v>
       </c>
       <c r="C26">
-        <v>100014.6484375</v>
+        <v>100003.4027099609</v>
       </c>
       <c r="D26">
-        <v>-14.6484375</v>
+        <v>-3.4027099609375</v>
       </c>
       <c r="E26">
-        <v>12682.54386054145</v>
+        <v>11330.08239169916</v>
       </c>
       <c r="F26">
-        <v>22514.95401295208</v>
+        <v>11257.47700647604</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -849,16 +849,16 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>100000.7629394531</v>
+        <v>100000.5187988281</v>
       </c>
       <c r="D27">
-        <v>-0.762939453125</v>
+        <v>-0.518798828125</v>
       </c>
       <c r="E27">
-        <v>1205.898106399209</v>
+        <v>1192.830309077903</v>
       </c>
       <c r="F27">
-        <v>2251.495401295208</v>
+        <v>1125.747700647604</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -866,16 +866,16 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>100000.4577636719</v>
+        <v>99999.42016601562</v>
       </c>
       <c r="D28">
-        <v>-0.457763671875</v>
+        <v>0.579833984375</v>
       </c>
       <c r="E28">
-        <v>111.2648257703492</v>
+        <v>133.3487985489724</v>
       </c>
       <c r="F28">
-        <v>225.1495401295208</v>
+        <v>112.5747700647604</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -883,16 +883,16 @@
         <v>20</v>
       </c>
       <c r="C29">
-        <v>100002.2888183594</v>
+        <v>100001.1444091797</v>
       </c>
       <c r="D29">
-        <v>-2.288818359375</v>
+        <v>-1.1444091796875</v>
       </c>
       <c r="E29">
-        <v>44.09671281323288</v>
+        <v>51.12835080237002</v>
       </c>
       <c r="F29">
-        <v>22.51495401295207</v>
+        <v>11.25747700647604</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -900,16 +900,16 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>100004.8828125</v>
+        <v>100004.7607421875</v>
       </c>
       <c r="D30">
-        <v>-4.8828125</v>
+        <v>-4.7607421875</v>
       </c>
       <c r="E30">
-        <v>17.30942966962101</v>
+        <v>18.70476089798294</v>
       </c>
       <c r="F30">
-        <v>2.251495401295208</v>
+        <v>1.125747700647604</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0.2251495401295208</v>
+        <v>0.1125747700647604</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -943,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0.02251495401295208</v>
+        <v>0.01125747700647604</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0.002251495401295208</v>
+        <v>0.001125747700647604</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -971,16 +971,16 @@
         <v>-10</v>
       </c>
       <c r="C34">
-        <v>99991.53137207031</v>
+        <v>100006.7443847656</v>
       </c>
       <c r="D34">
-        <v>8.4686279296875</v>
+        <v>-6.744384765625</v>
       </c>
       <c r="E34">
-        <v>9857.78487202796</v>
+        <v>11621.28151022457</v>
       </c>
       <c r="F34">
-        <v>22514.95401295208</v>
+        <v>11257.47700647604</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -988,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>100002.555847168</v>
+        <v>100001.8005371094</v>
       </c>
       <c r="D35">
-        <v>-2.55584716796875</v>
+        <v>-1.800537109375</v>
       </c>
       <c r="E35">
-        <v>1323.564304979612</v>
+        <v>1079.254169334043</v>
       </c>
       <c r="F35">
-        <v>2251.495401295208</v>
+        <v>1125.747700647604</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1005,16 +1005,16 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>99999.50408935547</v>
+        <v>100000.3280639648</v>
       </c>
       <c r="D36">
-        <v>0.49591064453125</v>
+        <v>-0.32806396484375</v>
       </c>
       <c r="E36">
-        <v>121.6643005421366</v>
+        <v>115.8006745646964</v>
       </c>
       <c r="F36">
-        <v>225.1495401295208</v>
+        <v>112.5747700647604</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1022,16 +1022,16 @@
         <v>20</v>
       </c>
       <c r="C37">
-        <v>100000</v>
+        <v>100000.1640319824</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>-0.164031982421875</v>
       </c>
       <c r="E37">
-        <v>10.87718916059744</v>
+        <v>12.53811369843043</v>
       </c>
       <c r="F37">
-        <v>22.51495401295207</v>
+        <v>11.25747700647604</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1039,16 +1039,16 @@
         <v>30</v>
       </c>
       <c r="C38">
-        <v>99999.88555908203</v>
+        <v>99999.80545043945</v>
       </c>
       <c r="D38">
-        <v>0.11444091796875</v>
+        <v>0.194549560546875</v>
       </c>
       <c r="E38">
-        <v>3.426314585588195</v>
+        <v>3.338623041467922</v>
       </c>
       <c r="F38">
-        <v>2.251495401295208</v>
+        <v>1.125747700647604</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1056,16 +1056,16 @@
         <v>40</v>
       </c>
       <c r="C39">
-        <v>99998.93188476562</v>
+        <v>99998.96240234375</v>
       </c>
       <c r="D39">
-        <v>1.068115234375</v>
+        <v>1.03759765625</v>
       </c>
       <c r="E39">
-        <v>1.552204291025798</v>
+        <v>1.625852422551946</v>
       </c>
       <c r="F39">
-        <v>0.2251495401295208</v>
+        <v>0.1125747700647604</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.02251495401295208</v>
+        <v>0.01125747700647604</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.002251495401295208</v>
+        <v>0.001125747700647604</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1110,16 +1110,16 @@
         <v>-10</v>
       </c>
       <c r="C42">
-        <v>99973.58322143555</v>
+        <v>100000.1211166382</v>
       </c>
       <c r="D42">
-        <v>26.41677856445312</v>
+        <v>-0.1211166381835938</v>
       </c>
       <c r="E42">
-        <v>13187.07603272145</v>
+        <v>11253.58350410981</v>
       </c>
       <c r="F42">
-        <v>22514.95401295208</v>
+        <v>11257.47700647604</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1127,16 +1127,16 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>100000.0190734863</v>
+        <v>100000.5912780762</v>
       </c>
       <c r="D43">
-        <v>-0.019073486328125</v>
+        <v>-0.591278076171875</v>
       </c>
       <c r="E43">
-        <v>956.2882960472971</v>
+        <v>1169.919360054282</v>
       </c>
       <c r="F43">
-        <v>2251.495401295208</v>
+        <v>1125.747700647604</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1144,16 +1144,16 @@
         <v>10</v>
       </c>
       <c r="C44">
-        <v>100000.0858306885</v>
+        <v>99999.47071075439</v>
       </c>
       <c r="D44">
-        <v>-0.0858306884765625</v>
+        <v>0.5292892456054688</v>
       </c>
       <c r="E44">
-        <v>104.0258910212986</v>
+        <v>109.8631135125932</v>
       </c>
       <c r="F44">
-        <v>225.1495401295208</v>
+        <v>112.5747700647604</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1161,16 +1161,16 @@
         <v>20</v>
       </c>
       <c r="C45">
-        <v>100000.524520874</v>
+        <v>99999.84645843506</v>
       </c>
       <c r="D45">
-        <v>-0.5245208740234375</v>
+        <v>0.1535415649414062</v>
       </c>
       <c r="E45">
-        <v>13.71361834415696</v>
+        <v>11.489566451848</v>
       </c>
       <c r="F45">
-        <v>22.51495401295207</v>
+        <v>11.25747700647604</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1178,16 +1178,16 @@
         <v>30</v>
       </c>
       <c r="C46">
-        <v>99999.91416931152</v>
+        <v>100000.0305175781</v>
       </c>
       <c r="D46">
-        <v>0.0858306884765625</v>
+        <v>-0.030517578125</v>
       </c>
       <c r="E46">
-        <v>1.276875440398175</v>
+        <v>1.165842930147717</v>
       </c>
       <c r="F46">
-        <v>2.251495401295208</v>
+        <v>1.125747700647604</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1195,16 +1195,16 @@
         <v>40</v>
       </c>
       <c r="C47">
-        <v>99999.96185302734</v>
+        <v>100000.036239624</v>
       </c>
       <c r="D47">
-        <v>0.03814697265625</v>
+        <v>-0.0362396240234375</v>
       </c>
       <c r="E47">
-        <v>0.2263631257745955</v>
+        <v>0.2230091933608503</v>
       </c>
       <c r="F47">
-        <v>0.2251495401295208</v>
+        <v>0.1125747700647604</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1212,16 +1212,16 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>100000.2002716064</v>
+        <v>100000.2145767212</v>
       </c>
       <c r="D48">
-        <v>-0.2002716064453125</v>
+        <v>-0.2145767211914062</v>
       </c>
       <c r="E48">
-        <v>0.1413850854574279</v>
+        <v>0.1314397373057723</v>
       </c>
       <c r="F48">
-        <v>0.02251495401295208</v>
+        <v>0.01125747700647604</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -1229,16 +1229,16 @@
         <v>60</v>
       </c>
       <c r="C49">
-        <v>100000.3814697266</v>
+        <v>100000.3786087036</v>
       </c>
       <c r="D49">
-        <v>-0.3814697265625</v>
+        <v>-0.3786087036132812</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>0.002723021674677506</v>
       </c>
       <c r="F49">
-        <v>0.002251495401295208</v>
+        <v>0.001125747700647604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added phase calcs to auto.py
</commit_message>
<xml_diff>
--- a/innafor.xlsx
+++ b/innafor.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FFT Length</t>
   </si>
@@ -22,16 +22,28 @@
     <t>SNR [dB]</t>
   </si>
   <si>
-    <t>Mean estimated</t>
+    <t>Mean estimated frequency [Hz]</t>
   </si>
   <si>
-    <t>Mean error</t>
+    <t>Mean frequency error [Hz]</t>
   </si>
   <si>
-    <t>Variance</t>
+    <t>Frequency variance [Hz^2]</t>
   </si>
   <si>
-    <t>CRLB [Hz^2]</t>
+    <t>Frequency CRLB [Hz^2]</t>
+  </si>
+  <si>
+    <t>Mean estimated phase [rad]</t>
+  </si>
+  <si>
+    <t>Mean phase error [rad]</t>
+  </si>
+  <si>
+    <t>Phase variance [rad^2]</t>
+  </si>
+  <si>
+    <t>Phase CRLB [rad^2]</t>
   </si>
   <si>
     <t>1024</t>
@@ -381,13 +393,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,28 +418,52 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>-10</v>
       </c>
       <c r="C2">
-        <v>99787.109375</v>
+        <v>99707.03125</v>
       </c>
       <c r="D2">
-        <v>212.890625</v>
+        <v>292.96875</v>
       </c>
       <c r="E2">
-        <v>142121.338868165</v>
+        <v>95367.431640625</v>
       </c>
       <c r="F2">
         <v>11257.47700647604</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>0.4244357951296026</v>
+      </c>
+      <c r="H2">
+        <v>-0.03173671343087849</v>
+      </c>
+      <c r="I2">
+        <v>0.006986436251629604</v>
+      </c>
+      <c r="J2">
+        <v>0.009746588693957114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="B3">
         <v>0</v>
       </c>
@@ -443,8 +479,20 @@
       <c r="F3">
         <v>1125.747700647604</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>0.3849124711463262</v>
+      </c>
+      <c r="H3">
+        <v>0.007786610552397977</v>
+      </c>
+      <c r="I3">
+        <v>0.0005895149415695069</v>
+      </c>
+      <c r="J3">
+        <v>0.0009746588693957114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="B4">
         <v>10</v>
       </c>
@@ -460,8 +508,20 @@
       <c r="F4">
         <v>112.5747700647604</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0.3869535216095011</v>
+      </c>
+      <c r="H4">
+        <v>0.005745560089223056</v>
+      </c>
+      <c r="I4">
+        <v>5.443919164565485E-05</v>
+      </c>
+      <c r="J4">
+        <v>9.746588693957116E-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5">
         <v>20</v>
       </c>
@@ -477,8 +537,20 @@
       <c r="F5">
         <v>11.25747700647604</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>0.3935103349775683</v>
+      </c>
+      <c r="H5">
+        <v>-0.0008112532788441095</v>
+      </c>
+      <c r="I5">
+        <v>5.870248267112402E-06</v>
+      </c>
+      <c r="J5">
+        <v>9.746588693957114E-06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6">
         <v>30</v>
       </c>
@@ -494,8 +566,20 @@
       <c r="F6">
         <v>1.125747700647604</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>0.3926106599128618</v>
+      </c>
+      <c r="H6">
+        <v>8.842178586230265E-05</v>
+      </c>
+      <c r="I6">
+        <v>1.634039436763756E-06</v>
+      </c>
+      <c r="J6">
+        <v>9.746588693957115E-07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="B7">
         <v>40</v>
       </c>
@@ -511,8 +595,20 @@
       <c r="F7">
         <v>0.1125747700647604</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>0.3925484514057116</v>
+      </c>
+      <c r="H7">
+        <v>0.0001506302930125436</v>
+      </c>
+      <c r="I7">
+        <v>1.363890024806207E-07</v>
+      </c>
+      <c r="J7">
+        <v>9.746588693957116E-08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="B8">
         <v>50</v>
       </c>
@@ -528,8 +624,20 @@
       <c r="F8">
         <v>0.01125747700647604</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>0.3926618152178197</v>
+      </c>
+      <c r="H8">
+        <v>3.72664809043799E-05</v>
+      </c>
+      <c r="I8">
+        <v>4.371333444314124E-09</v>
+      </c>
+      <c r="J8">
+        <v>9.746588693957116E-09</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9">
         <v>60</v>
       </c>
@@ -545,62 +653,110 @@
       <c r="F9">
         <v>0.001125747700647604</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0.3927007885041309</v>
+      </c>
+      <c r="H9">
+        <v>-1.706805406787026E-06</v>
+      </c>
+      <c r="I9">
+        <v>6.888043657628275E-10</v>
+      </c>
+      <c r="J9">
+        <v>9.746588693957116E-10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>-10</v>
       </c>
       <c r="C10">
-        <v>99991.69921875</v>
+        <v>100048.828125</v>
       </c>
       <c r="D10">
-        <v>8.30078125</v>
+        <v>-48.828125</v>
       </c>
       <c r="E10">
-        <v>19309.99564933586</v>
+        <v>10596.38129340278</v>
       </c>
       <c r="F10">
         <v>11257.47700647604</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>0.3466482451438087</v>
+      </c>
+      <c r="H10">
+        <v>0.04605083655491541</v>
+      </c>
+      <c r="I10">
+        <v>0.005245439678475339</v>
+      </c>
+      <c r="J10">
+        <v>0.009746588693957114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>100040.771484375</v>
+        <v>100048.828125</v>
       </c>
       <c r="D11">
-        <v>-40.771484375</v>
+        <v>-48.828125</v>
       </c>
       <c r="E11">
-        <v>10662.66834079563</v>
+        <v>10596.38129340278</v>
       </c>
       <c r="F11">
         <v>1125.747700647604</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>0.3866679943603236</v>
+      </c>
+      <c r="H11">
+        <v>0.006031087338400576</v>
+      </c>
+      <c r="I11">
+        <v>0.0004417157432207876</v>
+      </c>
+      <c r="J11">
+        <v>0.0009746588693957114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>100094.970703125</v>
+        <v>100097.65625</v>
       </c>
       <c r="D12">
-        <v>-94.970703125</v>
+        <v>-97.65625</v>
       </c>
       <c r="E12">
-        <v>649.0880185300047</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>112.5747700647604</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>0.3883884376352533</v>
+      </c>
+      <c r="H12">
+        <v>0.004310644063470842</v>
+      </c>
+      <c r="I12">
+        <v>7.630418125147208E-05</v>
+      </c>
+      <c r="J12">
+        <v>9.746588693957116E-05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13">
         <v>20</v>
       </c>
@@ -616,8 +772,20 @@
       <c r="F13">
         <v>11.25747700647604</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>0.3934068937716507</v>
+      </c>
+      <c r="H13">
+        <v>-0.0007078120729265336</v>
+      </c>
+      <c r="I13">
+        <v>8.173233407869795E-06</v>
+      </c>
+      <c r="J13">
+        <v>9.746588693957114E-06</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14">
         <v>30</v>
       </c>
@@ -633,8 +801,20 @@
       <c r="F14">
         <v>1.125747700647604</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>0.392457212450293</v>
+      </c>
+      <c r="H14">
+        <v>0.0002418692484311147</v>
+      </c>
+      <c r="I14">
+        <v>5.519331425412203E-07</v>
+      </c>
+      <c r="J14">
+        <v>9.746588693957115E-07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15">
         <v>40</v>
       </c>
@@ -650,8 +830,20 @@
       <c r="F15">
         <v>0.1125747700647604</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>0.3927115534081193</v>
+      </c>
+      <c r="H15">
+        <v>-1.247170939513986E-05</v>
+      </c>
+      <c r="I15">
+        <v>1.322134804060803E-07</v>
+      </c>
+      <c r="J15">
+        <v>9.746588693957116E-08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="B16">
         <v>50</v>
       </c>
@@ -667,8 +859,20 @@
       <c r="F16">
         <v>0.01125747700647604</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>0.3926826377733138</v>
+      </c>
+      <c r="H16">
+        <v>1.644392541031436E-05</v>
+      </c>
+      <c r="I16">
+        <v>4.04745463162938E-09</v>
+      </c>
+      <c r="J16">
+        <v>9.746588693957116E-09</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="B17">
         <v>60</v>
       </c>
@@ -684,79 +888,139 @@
       <c r="F17">
         <v>0.001125747700647604</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>0.3926804878837548</v>
+      </c>
+      <c r="H17">
+        <v>1.859381496934209E-05</v>
+      </c>
+      <c r="I17">
+        <v>1.783628333244188E-09</v>
+      </c>
+      <c r="J17">
+        <v>9.746588693957116E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>-10</v>
       </c>
       <c r="C18">
-        <v>99999.51171875</v>
+        <v>100006.103515625</v>
       </c>
       <c r="D18">
-        <v>0.48828125</v>
+        <v>-6.103515625</v>
       </c>
       <c r="E18">
-        <v>11449.34225607443</v>
+        <v>3518.329726325141</v>
       </c>
       <c r="F18">
         <v>11257.47700647604</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>0.3887585709096021</v>
+      </c>
+      <c r="H18">
+        <v>0.003940510789122054</v>
+      </c>
+      <c r="I18">
+        <v>0.01174838918815676</v>
+      </c>
+      <c r="J18">
+        <v>0.009746588693957114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>100000.0610351562</v>
+        <v>100000</v>
       </c>
       <c r="D19">
-        <v>-0.06103515625</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1552.014111040591</v>
+        <v>993.4107462565104</v>
       </c>
       <c r="F19">
         <v>1125.747700647604</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>0.3875625048859843</v>
+      </c>
+      <c r="H19">
+        <v>0.005136576812739863</v>
+      </c>
+      <c r="I19">
+        <v>0.001331486649372985</v>
+      </c>
+      <c r="J19">
+        <v>0.0009746588693957114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20">
-        <v>99993.5302734375</v>
+        <v>99981.689453125</v>
       </c>
       <c r="D20">
-        <v>6.4697265625</v>
+        <v>18.310546875</v>
       </c>
       <c r="E20">
-        <v>774.0101656756243</v>
+        <v>372.5290298461914</v>
       </c>
       <c r="F20">
         <v>112.5747700647604</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>0.3915069606370982</v>
+      </c>
+      <c r="H20">
+        <v>0.001192121061625911</v>
+      </c>
+      <c r="I20">
+        <v>0.0001314012356066161</v>
+      </c>
+      <c r="J20">
+        <v>9.746588693957116E-05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21">
-        <v>99977.72216796875</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D21">
-        <v>22.27783203125</v>
+        <v>24.4140625</v>
       </c>
       <c r="E21">
-        <v>125.9476274580092</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>11.25747700647604</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>0.3929500916699218</v>
+      </c>
+      <c r="H21">
+        <v>-0.0002510099711977187</v>
+      </c>
+      <c r="I21">
+        <v>5.693439189550872E-06</v>
+      </c>
+      <c r="J21">
+        <v>9.746588693957114E-06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="B22">
         <v>30</v>
       </c>
@@ -772,8 +1036,20 @@
       <c r="F22">
         <v>1.125747700647604</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>0.3930804975908629</v>
+      </c>
+      <c r="H22">
+        <v>-0.0003814158921387367</v>
+      </c>
+      <c r="I22">
+        <v>7.896082796645321E-07</v>
+      </c>
+      <c r="J22">
+        <v>9.746588693957115E-07</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="B23">
         <v>40</v>
       </c>
@@ -789,8 +1065,20 @@
       <c r="F23">
         <v>0.1125747700647604</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>0.3927390319885239</v>
+      </c>
+      <c r="H23">
+        <v>-3.995028979977833E-05</v>
+      </c>
+      <c r="I23">
+        <v>9.378432543627663E-08</v>
+      </c>
+      <c r="J23">
+        <v>9.746588693957116E-08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="B24">
         <v>50</v>
       </c>
@@ -806,8 +1094,20 @@
       <c r="F24">
         <v>0.01125747700647604</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>0.3927563081587463</v>
+      </c>
+      <c r="H24">
+        <v>-5.722646002223053E-05</v>
+      </c>
+      <c r="I24">
+        <v>4.081075203144876E-09</v>
+      </c>
+      <c r="J24">
+        <v>9.746588693957116E-09</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="B25">
         <v>60</v>
       </c>
@@ -823,96 +1123,168 @@
       <c r="F25">
         <v>0.001125747700647604</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>0.3926790277776924</v>
+      </c>
+      <c r="H25">
+        <v>2.005392103174852E-05</v>
+      </c>
+      <c r="I25">
+        <v>5.429763571385168E-10</v>
+      </c>
+      <c r="J25">
+        <v>9.746588693957116E-10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>-10</v>
       </c>
       <c r="C26">
-        <v>100003.4027099609</v>
+        <v>99945.068359375</v>
       </c>
       <c r="D26">
-        <v>-3.4027099609375</v>
+        <v>54.931640625</v>
       </c>
       <c r="E26">
-        <v>11330.08239169916</v>
+        <v>7191.879881752862</v>
       </c>
       <c r="F26">
         <v>11257.47700647604</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>0.4381419954231404</v>
+      </c>
+      <c r="H26">
+        <v>-0.04544291372441629</v>
+      </c>
+      <c r="I26">
+        <v>0.01120653478205223</v>
+      </c>
+      <c r="J26">
+        <v>0.009746588693957114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>100000.5187988281</v>
+        <v>100004.5776367188</v>
       </c>
       <c r="D27">
-        <v>-0.518798828125</v>
+        <v>-4.57763671875</v>
       </c>
       <c r="E27">
-        <v>1192.830309077903</v>
+        <v>851.125352912479</v>
       </c>
       <c r="F27">
         <v>1125.747700647604</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>0.3988132893836333</v>
+      </c>
+      <c r="H27">
+        <v>-0.00611420768490914</v>
+      </c>
+      <c r="I27">
+        <v>0.001114595261036145</v>
+      </c>
+      <c r="J27">
+        <v>0.0009746588693957114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="B28">
         <v>10</v>
       </c>
       <c r="C28">
-        <v>99999.42016601562</v>
+        <v>99996.9482421875</v>
       </c>
       <c r="D28">
-        <v>0.579833984375</v>
+        <v>3.0517578125</v>
       </c>
       <c r="E28">
-        <v>133.3487985489724</v>
+        <v>113.8283146752252</v>
       </c>
       <c r="F28">
         <v>112.5747700647604</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>0.3941083077768128</v>
+      </c>
+      <c r="H28">
+        <v>-0.001409226078088654</v>
+      </c>
+      <c r="I28">
+        <v>9.747932965134797E-05</v>
+      </c>
+      <c r="J28">
+        <v>9.746588693957116E-05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="B29">
         <v>20</v>
       </c>
       <c r="C29">
-        <v>100001.1444091797</v>
+        <v>100001.5258789062</v>
       </c>
       <c r="D29">
-        <v>-1.1444091796875</v>
+        <v>-1.52587890625</v>
       </c>
       <c r="E29">
-        <v>51.12835080237002</v>
+        <v>54.32715018590292</v>
       </c>
       <c r="F29">
         <v>11.25747700647604</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>0.3915354747878423</v>
+      </c>
+      <c r="H29">
+        <v>0.001163606910881843</v>
+      </c>
+      <c r="I29">
+        <v>4.922915801565851E-06</v>
+      </c>
+      <c r="J29">
+        <v>9.746588693957114E-06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="B30">
         <v>30</v>
       </c>
       <c r="C30">
-        <v>100004.7607421875</v>
+        <v>100003.0517578125</v>
       </c>
       <c r="D30">
-        <v>-4.7607421875</v>
+        <v>-3.0517578125</v>
       </c>
       <c r="E30">
-        <v>18.70476089798294</v>
+        <v>41.3921144273546</v>
       </c>
       <c r="F30">
         <v>1.125747700647604</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>0.3927430499391708</v>
+      </c>
+      <c r="H30">
+        <v>-4.396824044665682E-05</v>
+      </c>
+      <c r="I30">
+        <v>6.57501364206769E-07</v>
+      </c>
+      <c r="J30">
+        <v>9.746588693957115E-07</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="B31">
         <v>40</v>
       </c>
@@ -928,8 +1300,20 @@
       <c r="F31">
         <v>0.1125747700647604</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>0.3928095115080135</v>
+      </c>
+      <c r="H31">
+        <v>-0.0001104298092893918</v>
+      </c>
+      <c r="I31">
+        <v>2.898508693536543E-08</v>
+      </c>
+      <c r="J31">
+        <v>9.746588693957116E-08</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="B32">
         <v>50</v>
       </c>
@@ -945,8 +1329,20 @@
       <c r="F32">
         <v>0.01125747700647604</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>0.3927675108123639</v>
+      </c>
+      <c r="H32">
+        <v>-6.84291136397841E-05</v>
+      </c>
+      <c r="I32">
+        <v>7.96387056330015E-09</v>
+      </c>
+      <c r="J32">
+        <v>9.746588693957116E-09</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="B33">
         <v>60</v>
       </c>
@@ -962,113 +1358,197 @@
       <c r="F33">
         <v>0.001125747700647604</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>0.392679851293281</v>
+      </c>
+      <c r="H33">
+        <v>1.923040544315469E-05</v>
+      </c>
+      <c r="I33">
+        <v>1.228544542848966E-09</v>
+      </c>
+      <c r="J33">
+        <v>9.746588693957116E-10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B34">
         <v>-10</v>
       </c>
       <c r="C34">
-        <v>100006.7443847656</v>
+        <v>99975.5859375</v>
       </c>
       <c r="D34">
-        <v>-6.744384765625</v>
+        <v>24.4140625</v>
       </c>
       <c r="E34">
-        <v>11621.28151022457</v>
+        <v>21785.83397633499</v>
       </c>
       <c r="F34">
         <v>11257.47700647604</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>0.377802779954863</v>
+      </c>
+      <c r="H34">
+        <v>0.01489630174386115</v>
+      </c>
+      <c r="I34">
+        <v>0.007825375294778194</v>
+      </c>
+      <c r="J34">
+        <v>0.009746588693957114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>100001.8005371094</v>
+        <v>99992.75207519531</v>
       </c>
       <c r="D35">
-        <v>-1.800537109375</v>
+        <v>7.2479248046875</v>
       </c>
       <c r="E35">
-        <v>1079.254169334043</v>
+        <v>1475.402516209417</v>
       </c>
       <c r="F35">
         <v>1125.747700647604</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>0.3885919792028614</v>
+      </c>
+      <c r="H35">
+        <v>0.004107102495862702</v>
+      </c>
+      <c r="I35">
+        <v>0.0009132882707293078</v>
+      </c>
+      <c r="J35">
+        <v>0.0009746588693957114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="B36">
         <v>10</v>
       </c>
       <c r="C36">
-        <v>100000.3280639648</v>
+        <v>99998.85559082031</v>
       </c>
       <c r="D36">
-        <v>-0.32806396484375</v>
+        <v>1.1444091796875</v>
       </c>
       <c r="E36">
-        <v>115.8006745646964</v>
+        <v>134.0393080479569</v>
       </c>
       <c r="F36">
         <v>112.5747700647604</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>0.3886927975782652</v>
+      </c>
+      <c r="H36">
+        <v>0.004006284120458936</v>
+      </c>
+      <c r="I36">
+        <v>4.009326117276929E-05</v>
+      </c>
+      <c r="J36">
+        <v>9.746588693957116E-05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="B37">
         <v>20</v>
       </c>
       <c r="C37">
-        <v>100000.1640319824</v>
+        <v>100001.1444091797</v>
       </c>
       <c r="D37">
-        <v>-0.164031982421875</v>
+        <v>-1.1444091796875</v>
       </c>
       <c r="E37">
-        <v>12.53811369843043</v>
+        <v>13.09672370553017</v>
       </c>
       <c r="F37">
         <v>11.25747700647604</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>0.3932885757629283</v>
+      </c>
+      <c r="H37">
+        <v>-0.000589494064204188</v>
+      </c>
+      <c r="I37">
+        <v>9.23582903733572E-06</v>
+      </c>
+      <c r="J37">
+        <v>9.746588693957114E-06</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="B38">
         <v>30</v>
       </c>
       <c r="C38">
-        <v>99999.80545043945</v>
+        <v>100000</v>
       </c>
       <c r="D38">
-        <v>0.194549560546875</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>3.338623041467922</v>
+        <v>3.880510727564494</v>
       </c>
       <c r="F38">
         <v>1.125747700647604</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>0.392393645547667</v>
+      </c>
+      <c r="H38">
+        <v>0.0003054361510570813</v>
+      </c>
+      <c r="I38">
+        <v>1.658313975009997E-06</v>
+      </c>
+      <c r="J38">
+        <v>9.746588693957115E-07</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="B39">
         <v>40</v>
       </c>
       <c r="C39">
-        <v>99998.96240234375</v>
+        <v>99999.23706054688</v>
       </c>
       <c r="D39">
-        <v>1.03759765625</v>
+        <v>0.762939453125</v>
       </c>
       <c r="E39">
-        <v>1.625852422551946</v>
+        <v>2.587007151709662</v>
       </c>
       <c r="F39">
         <v>0.1125747700647604</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>0.3926994969701121</v>
+      </c>
+      <c r="H39">
+        <v>-4.152713879712611E-07</v>
+      </c>
+      <c r="I39">
+        <v>1.3198528280054E-07</v>
+      </c>
+      <c r="J39">
+        <v>9.746588693957116E-08</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="B40">
         <v>50</v>
       </c>
@@ -1084,8 +1564,20 @@
       <c r="F40">
         <v>0.01125747700647604</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>0.3927485314761216</v>
+      </c>
+      <c r="H40">
+        <v>-4.944977739748113E-05</v>
+      </c>
+      <c r="I40">
+        <v>2.855403667911182E-09</v>
+      </c>
+      <c r="J40">
+        <v>9.746588693957116E-09</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="B41">
         <v>60</v>
       </c>
@@ -1101,144 +1593,252 @@
       <c r="F41">
         <v>0.001125747700647604</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>0.3926937055226744</v>
+      </c>
+      <c r="H41">
+        <v>5.37617604978724E-06</v>
+      </c>
+      <c r="I41">
+        <v>8.168450733329186E-10</v>
+      </c>
+      <c r="J41">
+        <v>9.746588693957116E-10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B42">
         <v>-10</v>
       </c>
       <c r="C42">
-        <v>100000.1211166382</v>
+        <v>100016.8800354004</v>
       </c>
       <c r="D42">
-        <v>-0.1211166381835938</v>
+        <v>-16.88003540039062</v>
       </c>
       <c r="E42">
-        <v>11253.58350410981</v>
+        <v>6430.946086766198</v>
       </c>
       <c r="F42">
         <v>11257.47700647604</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>0.3508551874257532</v>
+      </c>
+      <c r="H42">
+        <v>0.04184389427297099</v>
+      </c>
+      <c r="I42">
+        <v>0.004944576012999051</v>
+      </c>
+      <c r="J42">
+        <v>0.009746588693957114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>100000.5912780762</v>
+        <v>99990.55862426758</v>
       </c>
       <c r="D43">
-        <v>-0.591278076171875</v>
+        <v>9.441375732421875</v>
       </c>
       <c r="E43">
-        <v>1169.919360054282</v>
+        <v>1914.799617629291</v>
       </c>
       <c r="F43">
         <v>1125.747700647604</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>0.3794677356901841</v>
+      </c>
+      <c r="H43">
+        <v>0.01323134600854001</v>
+      </c>
+      <c r="I43">
+        <v>0.001085954757588375</v>
+      </c>
+      <c r="J43">
+        <v>0.0009746588693957114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="B44">
         <v>10</v>
       </c>
       <c r="C44">
-        <v>99999.47071075439</v>
+        <v>99994.85015869141</v>
       </c>
       <c r="D44">
-        <v>0.5292892456054688</v>
+        <v>5.14984130859375</v>
       </c>
       <c r="E44">
-        <v>109.8631135125932</v>
+        <v>218.4404163724846</v>
       </c>
       <c r="F44">
         <v>112.5747700647604</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>0.3869853410566976</v>
+      </c>
+      <c r="H44">
+        <v>0.005713740642026494</v>
+      </c>
+      <c r="I44">
+        <v>7.617394437975063E-05</v>
+      </c>
+      <c r="J44">
+        <v>9.746588693957116E-05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="B45">
         <v>20</v>
       </c>
       <c r="C45">
-        <v>99999.84645843506</v>
+        <v>99999.90463256836</v>
       </c>
       <c r="D45">
-        <v>0.1535415649414062</v>
+        <v>0.095367431640625</v>
       </c>
       <c r="E45">
-        <v>11.489566451848</v>
+        <v>10.1560241697977</v>
       </c>
       <c r="F45">
         <v>11.25747700647604</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>0.394396736201254</v>
+      </c>
+      <c r="H45">
+        <v>-0.00169765450252985</v>
+      </c>
+      <c r="I45">
+        <v>3.66270399081424E-06</v>
+      </c>
+      <c r="J45">
+        <v>9.746588693957114E-06</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="B46">
         <v>30</v>
       </c>
       <c r="C46">
-        <v>100000.0305175781</v>
+        <v>99999.80926513672</v>
       </c>
       <c r="D46">
-        <v>-0.030517578125</v>
+        <v>0.19073486328125</v>
       </c>
       <c r="E46">
-        <v>1.165842930147717</v>
+        <v>1.85941139029132</v>
       </c>
       <c r="F46">
         <v>1.125747700647604</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>0.3925366747085114</v>
+      </c>
+      <c r="H46">
+        <v>0.0001624069902127323</v>
+      </c>
+      <c r="I46">
+        <v>6.327499733615374E-07</v>
+      </c>
+      <c r="J46">
+        <v>9.746588693957115E-07</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="B47">
         <v>40</v>
       </c>
       <c r="C47">
-        <v>100000.036239624</v>
+        <v>100000.0953674316</v>
       </c>
       <c r="D47">
-        <v>-0.0362396240234375</v>
+        <v>-0.095367431640625</v>
       </c>
       <c r="E47">
-        <v>0.2230091933608503</v>
+        <v>0.2122154304136833</v>
       </c>
       <c r="F47">
         <v>0.1125747700647604</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>0.392775511526365</v>
+      </c>
+      <c r="H47">
+        <v>-7.642982764082817E-05</v>
+      </c>
+      <c r="I47">
+        <v>1.361923361820592E-07</v>
+      </c>
+      <c r="J47">
+        <v>9.746588693957116E-08</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="B48">
         <v>50</v>
       </c>
       <c r="C48">
-        <v>100000.2145767212</v>
+        <v>100000.0953674316</v>
       </c>
       <c r="D48">
-        <v>-0.2145767211914062</v>
+        <v>-0.095367431640625</v>
       </c>
       <c r="E48">
-        <v>0.1314397373057723</v>
+        <v>0.2122154304136833</v>
       </c>
       <c r="F48">
         <v>0.01125747700647604</v>
       </c>
-    </row>
-    <row r="49" spans="2:6">
+      <c r="G48">
+        <v>0.3926645015835225</v>
+      </c>
+      <c r="H48">
+        <v>3.458011520166559E-05</v>
+      </c>
+      <c r="I48">
+        <v>7.64321546874377E-09</v>
+      </c>
+      <c r="J48">
+        <v>9.746588693957116E-09</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
       <c r="B49">
         <v>60</v>
       </c>
       <c r="C49">
-        <v>100000.3786087036</v>
+        <v>100000.2861022949</v>
       </c>
       <c r="D49">
-        <v>-0.3786087036132812</v>
+        <v>-0.286102294921875</v>
       </c>
       <c r="E49">
-        <v>0.002723021674677506</v>
+        <v>0.09094947017729282</v>
       </c>
       <c r="F49">
         <v>0.001125747700647604</v>
+      </c>
+      <c r="G49">
+        <v>0.3926797631151149</v>
+      </c>
+      <c r="H49">
+        <v>1.931858360920136E-05</v>
+      </c>
+      <c r="I49">
+        <v>1.480413333875358E-09</v>
+      </c>
+      <c r="J49">
+        <v>9.746588693957116E-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>